<commit_message>
perbaiki laporan Lipa 14
</commit_message>
<xml_diff>
--- a/hasil/2023_01_lipa_14.xlsx
+++ b/hasil/2023_01_lipa_14.xlsx
@@ -70,13 +70,13 @@
     <t>Mengetahui</t>
   </si>
   <si>
-    <t>Ternate , 17 Mei 2023</t>
+    <t>Ternate , 02 Agustus 2023</t>
   </si>
   <si>
     <t>Ketua Pengadilan Agama Ternate ,</t>
   </si>
   <si>
-    <t>Panitera,</t>
+    <t xml:space="preserve">Panitera, </t>
   </si>
   <si>
     <t>Drs. Djabir Sasole, M.H</t>
@@ -354,15 +354,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="164" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="164" fillId="2" borderId="2" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
@@ -838,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="18">
-        <v>70000000</v>
+        <v>90000000</v>
       </c>
       <c r="C9" s="18">
         <v>0</v>
@@ -853,7 +853,7 @@
         <v>100000</v>
       </c>
       <c r="G9" s="18">
-        <v>69900000</v>
+        <v>89900000</v>
       </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>

</xml_diff>